<commit_message>
Further work on thesis
</commit_message>
<xml_diff>
--- a/img/PerformanceComparison.xlsx
+++ b/img/PerformanceComparison.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moritz/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moritz/Desktop/git/sse-master-thesis/img/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8140008_{84DDBE74-8877-8D4F-A2FD-0BD4F3E81B61}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{02E7036B-FF6E-0344-96CF-B369B47AEA70}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="460" windowWidth="26160" windowHeight="14340"/>
+    <workbookView xWindow="1360" yWindow="460" windowWidth="25960" windowHeight="14340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PerformanceComparison" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">PerformanceComparison!$A$1:$KT$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">PerformanceComparison!$A$2:$KT$2</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">PerformanceComparison!$A$3:$KT$3</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -8166,6 +8161,2241 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Change</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>PerformanceComparison!$A$2:$KT$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="306"/>
+                <c:pt idx="0">
+                  <c:v>2928</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2480</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2289</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2783</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2466</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2540</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3198</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>9220</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3113</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3073</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3068</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>2186</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>2233</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>2092</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>2103</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>2405</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>2733</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>3224</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>2547</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>3027</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>2615</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>2159</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>2444</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>2879</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>2715</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>2294</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>2242</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>2224</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>2797</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>1740</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>2435</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>2447</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>2451</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>2659</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>2676</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>2706</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>2133</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>2172</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>2464</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>2563</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>2763</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>2545</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>2598</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>2589</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>2602</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="300">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="301">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="303">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="304">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>2596</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-67D4-1C43-9716-3CD3C3805730}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>VarChange</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>PerformanceComparison!$A$1:$KT$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="306"/>
+                <c:pt idx="0">
+                  <c:v>5663</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1194</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1941</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2234</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1785</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1339</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1372</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>2084</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>2090</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>1740</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>2280</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>2297</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>3174</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>2236</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>1224</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>3758</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>1320</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>1366</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>1928</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>1795</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>1228</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>2072</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>1307</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>3488</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="300">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="301">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="303">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="304">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-67D4-1C43-9716-3CD3C3805730}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="188500064"/>
+        <c:axId val="227813872"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="188500064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Commit-File-Nr</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="227813872"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="227813872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>time in s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="188500064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -8247,6 +10477,46 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -9834,20 +12104,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>112067</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9877,15 +12663,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>239067</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>20320</xdr:rowOff>
+      <xdr:colOff>340667</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9945,6 +12731,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>331716</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>189552</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>104297</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>35252</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Diagramm 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E013FE73-2251-9E40-A88F-D0C87777A524}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -10249,11 +13073,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:KT3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F2" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>